<commit_message>
fixed protocols files for VNC screen from ryo comments
</commit_message>
<xml_diff>
--- a/ProtocolFiles/EP_Bubble_v003p7.xlsx
+++ b/ProtocolFiles/EP_Bubble_v003p7.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bransonk\Documents\FlyBubbleParamFiles\ProtocolFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38745" yWindow="3255" windowWidth="22320" windowHeight="12525" tabRatio="500"/>
+    <workbookView xWindow="39675" yWindow="3255" windowWidth="22320" windowHeight="12525" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -400,7 +405,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -435,7 +440,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -650,7 +655,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -820,7 +825,7 @@
         <v>28</v>
       </c>
       <c r="B12" s="8">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>5</v>

</xml_diff>